<commit_message>
Mas cosas de la practica 5
</commit_message>
<xml_diff>
--- a/practica5/resumen.xlsx
+++ b/practica5/resumen.xlsx
@@ -19,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="48" uniqueCount="48">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="57" uniqueCount="57">
   <si>
     <t>Modelo</t>
   </si>
@@ -153,23 +153,50 @@
     <t>Acierto test %</t>
   </si>
   <si>
-    <t>Perceptron con 2 capa oculta (90, 70) 'relu,relu' y salida 'softmax' con earlystop 5 batch = 32</t>
-  </si>
-  <si>
-    <t>Perceptron con 2 capa oculta (90, 100) 'relu,relu' y salida 'softmax' con earlystop 5 batch = 32</t>
-  </si>
-  <si>
     <t>Perceptron con 2 capa oculta (90, 70) 'relu,relu' y salida 'softmax' con earlystop 5 batch = 32 funcion de coste = MSE</t>
   </si>
   <si>
     <t>Perceptron con 2 capa oculta (90, 100) 'relu,relu' y salida 'softmax' con earlystop 5 batch = 32 funcion de coste  = MSE</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Perceptron con 2 capas ocultas (100,100) 'relu,relu' y salida 'softmax' con batch = 16 </t>
+  </si>
+  <si>
+    <t>Perceptron de un solo nivel con salida 'relu'</t>
+  </si>
+  <si>
+    <t>Perceptron con 2 capas ocultas (100,100) 'relu,relu' y salida 'softmax' con batch = 16 y dropout (0,2) en las capas ocultas</t>
+  </si>
+  <si>
+    <t>Perceptron con 2 capas ocultas (100,100) 'relu,relu' y salida 'softmax' con batch = 16 y earlystop 5</t>
+  </si>
+  <si>
+    <t>Perceptron con 2 capas ocultas (100,100) 'relu,relu' y salida 'softmax' con batch = 16 y earlystop 3</t>
+  </si>
+  <si>
+    <t>Perceptron con 1 capa oculta (10000) 'relu' y salida 'softmax'</t>
+  </si>
+  <si>
+    <t>Perceptron con 2 capa oculta (90, 70) 'relu,relu' y salida 'softmax'  batch = 32</t>
+  </si>
+  <si>
+    <t>Perceptron con 2 capa oculta (90, 100) 'relu,relu' y salida 'softmax'  batch = 32</t>
+  </si>
+  <si>
+    <t>SOBREAJUSTE</t>
+  </si>
+  <si>
+    <t>Perceptron con 2 capas ocultas (100,100) 'relu,relu' y salida 'softmax' con batch = 16 dropout(0.2) y earlystop 5</t>
+  </si>
+  <si>
+    <t>Perceptron con 2 capas ocultas (100,100) 'relu,relu' y salida 'softmax' con batch = 16 dropout(0.2) y earlystop 3</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
-  <fonts count="19" x14ac:knownFonts="1">
+  <fonts count="20" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -306,6 +333,13 @@
     </font>
     <font>
       <sz val="11"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color theme="8"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
@@ -652,11 +686,13 @@
     <xf numFmtId="0" fontId="1" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="17" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="4">
+  <cellXfs count="6">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
-    <xf numFmtId="0" fontId="14" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="18" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="0" fontId="19" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="7" fillId="3" borderId="0" xfId="7"/>
   </cellXfs>
   <cellStyles count="42">
     <cellStyle name="20% - Énfasis1" xfId="19" builtinId="30" customBuiltin="1"/>
@@ -978,17 +1014,18 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:C56"/>
+  <dimension ref="A1:D54"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A37" workbookViewId="0">
-      <selection activeCell="C56" sqref="C56"/>
+    <sheetView tabSelected="1" topLeftCell="A46" workbookViewId="0">
+      <selection activeCell="E58" sqref="E58"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="98.109375" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="99.88671875" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="21.5546875" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="12.33203125" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="12.44140625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:3" x14ac:dyDescent="0.3">
@@ -1025,8 +1062,15 @@
       </c>
     </row>
     <row r="4" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="B4" s="1"/>
-      <c r="C4" s="1"/>
+      <c r="A4" t="s">
+        <v>47</v>
+      </c>
+      <c r="B4" s="1">
+        <v>55.3</v>
+      </c>
+      <c r="C4" s="1">
+        <v>54.25</v>
+      </c>
     </row>
     <row r="5" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A5" t="s">
@@ -1035,474 +1079,544 @@
       <c r="B5" s="1">
         <v>82.59</v>
       </c>
-      <c r="C5" s="1">
+      <c r="C5" s="3">
         <v>83.36</v>
       </c>
     </row>
     <row r="6" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="B6" s="1"/>
-      <c r="C6" s="1"/>
+      <c r="A6" t="s">
+        <v>4</v>
+      </c>
+      <c r="B6" s="1">
+        <v>9.8699999999999992</v>
+      </c>
+      <c r="C6" s="1">
+        <v>9.8000000000000007</v>
+      </c>
     </row>
     <row r="7" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A7" t="s">
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="B7" s="1">
-        <v>9.8699999999999992</v>
+        <v>91.57</v>
       </c>
       <c r="C7" s="1">
-        <v>9.8000000000000007</v>
+        <v>91.74</v>
       </c>
     </row>
     <row r="8" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A8" t="s">
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="B8" s="1">
-        <v>91.57</v>
+        <v>92.59</v>
       </c>
       <c r="C8" s="1">
-        <v>91.74</v>
+        <v>92.87</v>
       </c>
     </row>
     <row r="9" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A9" t="s">
-        <v>6</v>
+        <v>7</v>
       </c>
       <c r="B9" s="1">
-        <v>92.59</v>
+        <v>92.93</v>
       </c>
       <c r="C9" s="1">
-        <v>92.87</v>
+        <v>92.89</v>
       </c>
     </row>
     <row r="10" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A10" t="s">
-        <v>7</v>
+        <v>8</v>
       </c>
       <c r="B10" s="1">
-        <v>92.93</v>
+        <v>93.28</v>
       </c>
       <c r="C10" s="1">
-        <v>92.89</v>
+        <v>93.32</v>
       </c>
     </row>
     <row r="11" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A11" t="s">
-        <v>8</v>
+        <v>9</v>
       </c>
       <c r="B11" s="1">
-        <v>93.28</v>
+        <v>93.22</v>
       </c>
       <c r="C11" s="1">
-        <v>93.32</v>
+        <v>93.23</v>
       </c>
     </row>
     <row r="12" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A12" t="s">
-        <v>9</v>
+        <v>10</v>
       </c>
       <c r="B12" s="1">
-        <v>93.22</v>
+        <v>93.34</v>
       </c>
       <c r="C12" s="1">
-        <v>93.23</v>
+        <v>93.38</v>
       </c>
     </row>
     <row r="13" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A13" t="s">
-        <v>10</v>
+        <v>11</v>
       </c>
       <c r="B13" s="1">
-        <v>93.34</v>
+        <v>92</v>
       </c>
       <c r="C13" s="1">
-        <v>93.38</v>
+        <v>92.04</v>
+      </c>
+    </row>
+    <row r="14" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A14" t="s">
+        <v>12</v>
+      </c>
+      <c r="B14" s="1">
+        <v>92.15</v>
+      </c>
+      <c r="C14" s="1">
+        <v>92.12</v>
       </c>
     </row>
     <row r="15" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A15" t="s">
-        <v>11</v>
-      </c>
-      <c r="B15" s="1">
-        <v>92</v>
-      </c>
-      <c r="C15" s="1">
-        <v>92.04</v>
+        <v>13</v>
+      </c>
+      <c r="B15">
+        <v>92.31</v>
+      </c>
+      <c r="C15">
+        <v>92.46</v>
       </c>
     </row>
     <row r="16" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A16" t="s">
-        <v>12</v>
-      </c>
-      <c r="B16" s="1">
-        <v>92.15</v>
-      </c>
-      <c r="C16" s="1">
-        <v>92.12</v>
+        <v>14</v>
+      </c>
+      <c r="B16">
+        <v>92.44</v>
+      </c>
+      <c r="C16">
+        <v>92.64</v>
       </c>
     </row>
     <row r="17" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A17" t="s">
-        <v>13</v>
+        <v>15</v>
       </c>
       <c r="B17">
         <v>92.31</v>
       </c>
       <c r="C17">
-        <v>92.46</v>
+        <v>92.55</v>
       </c>
     </row>
     <row r="18" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A18" t="s">
-        <v>14</v>
+        <v>16</v>
       </c>
       <c r="B18">
-        <v>92.44</v>
+        <v>92.3</v>
       </c>
       <c r="C18">
-        <v>92.64</v>
+        <v>92.46</v>
       </c>
     </row>
     <row r="19" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A19" t="s">
-        <v>15</v>
+        <v>17</v>
       </c>
       <c r="B19">
-        <v>92.31</v>
+        <v>93.95</v>
       </c>
       <c r="C19">
-        <v>92.55</v>
+        <v>93.74</v>
       </c>
     </row>
     <row r="20" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A20" t="s">
-        <v>16</v>
+        <v>18</v>
       </c>
       <c r="B20">
-        <v>92.3</v>
+        <v>93.98</v>
       </c>
       <c r="C20">
-        <v>92.46</v>
+        <v>93.84</v>
+      </c>
+    </row>
+    <row r="21" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A21" t="s">
+        <v>19</v>
+      </c>
+      <c r="B21">
+        <v>93.84</v>
+      </c>
+      <c r="C21">
+        <v>94.03</v>
       </c>
     </row>
     <row r="22" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A22" t="s">
-        <v>17</v>
+        <v>20</v>
       </c>
       <c r="B22">
-        <v>93.95</v>
+        <v>93.81</v>
       </c>
       <c r="C22">
-        <v>93.74</v>
+        <v>93.78</v>
       </c>
     </row>
     <row r="23" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A23" t="s">
-        <v>18</v>
+        <v>21</v>
       </c>
       <c r="B23">
-        <v>93.98</v>
+        <v>93.78</v>
       </c>
       <c r="C23">
-        <v>93.84</v>
+        <v>93.7</v>
       </c>
     </row>
     <row r="24" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A24" t="s">
-        <v>19</v>
+        <v>22</v>
       </c>
       <c r="B24">
-        <v>93.84</v>
+        <v>94.04</v>
       </c>
       <c r="C24">
-        <v>94.03</v>
+        <v>94.05</v>
       </c>
     </row>
     <row r="25" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A25" t="s">
-        <v>20</v>
+        <v>23</v>
       </c>
       <c r="B25">
-        <v>93.81</v>
+        <v>93.68</v>
       </c>
       <c r="C25">
-        <v>93.78</v>
+        <v>93.62</v>
       </c>
     </row>
     <row r="26" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A26" t="s">
-        <v>21</v>
+        <v>24</v>
       </c>
       <c r="B26">
-        <v>93.78</v>
+        <v>94.21</v>
       </c>
       <c r="C26">
-        <v>93.7</v>
+        <v>94.16</v>
       </c>
     </row>
     <row r="27" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A27" t="s">
-        <v>22</v>
+        <v>25</v>
       </c>
       <c r="B27">
-        <v>94.04</v>
+        <v>94.24</v>
       </c>
       <c r="C27">
-        <v>94.05</v>
+        <v>93.99</v>
+      </c>
+    </row>
+    <row r="28" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A28" t="s">
+        <v>26</v>
+      </c>
+      <c r="B28">
+        <v>94.13</v>
+      </c>
+      <c r="C28">
+        <v>93.83</v>
       </c>
     </row>
     <row r="29" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A29" t="s">
-        <v>23</v>
+        <v>27</v>
       </c>
       <c r="B29">
-        <v>93.68</v>
+        <v>94.11</v>
       </c>
       <c r="C29">
-        <v>93.62</v>
+        <v>94.07</v>
       </c>
     </row>
     <row r="30" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A30" t="s">
-        <v>24</v>
+        <v>28</v>
       </c>
       <c r="B30">
-        <v>94.21</v>
+        <v>94.6</v>
       </c>
       <c r="C30">
-        <v>94.16</v>
+        <v>94.45</v>
       </c>
     </row>
     <row r="31" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A31" t="s">
-        <v>25</v>
+        <v>29</v>
       </c>
       <c r="B31">
-        <v>94.24</v>
+        <v>94.27</v>
       </c>
       <c r="C31">
-        <v>93.99</v>
+        <v>94.09</v>
       </c>
     </row>
     <row r="32" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A32" t="s">
-        <v>26</v>
+        <v>30</v>
       </c>
       <c r="B32">
-        <v>94.13</v>
+        <v>94.01</v>
       </c>
       <c r="C32">
-        <v>93.83</v>
+        <v>93.99</v>
       </c>
     </row>
     <row r="33" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A33" t="s">
-        <v>27</v>
+        <v>31</v>
       </c>
       <c r="B33">
-        <v>94.11</v>
+        <v>94.53</v>
       </c>
       <c r="C33">
-        <v>94.07</v>
+        <v>94.28</v>
       </c>
     </row>
     <row r="34" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A34" t="s">
-        <v>28</v>
+        <v>32</v>
       </c>
       <c r="B34">
-        <v>94.6</v>
+        <v>94.55</v>
       </c>
       <c r="C34">
-        <v>94.45</v>
+        <v>94.36</v>
+      </c>
+    </row>
+    <row r="35" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A35" t="s">
+        <v>33</v>
+      </c>
+      <c r="B35">
+        <v>94.54</v>
+      </c>
+      <c r="C35">
+        <v>94.49</v>
       </c>
     </row>
     <row r="36" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A36" t="s">
-        <v>29</v>
+        <v>34</v>
       </c>
       <c r="B36">
-        <v>94.27</v>
+        <v>94.55</v>
       </c>
       <c r="C36">
-        <v>94.09</v>
+        <v>94.44</v>
       </c>
     </row>
     <row r="37" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A37" t="s">
-        <v>30</v>
+        <v>35</v>
       </c>
       <c r="B37">
-        <v>94.01</v>
+        <v>94.04</v>
       </c>
       <c r="C37">
-        <v>93.99</v>
+        <v>93.8</v>
       </c>
     </row>
     <row r="38" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A38" t="s">
-        <v>31</v>
+      <c r="A38" s="2" t="s">
+        <v>36</v>
       </c>
       <c r="B38">
-        <v>94.53</v>
+        <v>94.49</v>
       </c>
       <c r="C38">
-        <v>94.28</v>
+        <v>94.22</v>
       </c>
     </row>
     <row r="39" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A39" t="s">
-        <v>32</v>
+        <v>37</v>
       </c>
       <c r="B39">
-        <v>94.55</v>
+        <v>94.58</v>
       </c>
       <c r="C39">
-        <v>94.36</v>
+        <v>94.46</v>
       </c>
     </row>
     <row r="40" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A40" t="s">
-        <v>33</v>
+      <c r="A40" s="4" t="s">
+        <v>38</v>
       </c>
       <c r="B40">
-        <v>94.54</v>
+        <v>94.83</v>
       </c>
       <c r="C40">
-        <v>94.49</v>
+        <v>94.64</v>
       </c>
     </row>
     <row r="41" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A41" t="s">
-        <v>34</v>
+        <v>39</v>
       </c>
       <c r="B41">
-        <v>94.55</v>
+        <v>94.63</v>
       </c>
       <c r="C41">
-        <v>94.44</v>
+        <v>94.37</v>
+      </c>
+    </row>
+    <row r="42" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A42" s="4" t="s">
+        <v>40</v>
+      </c>
+      <c r="B42">
+        <v>94.84</v>
+      </c>
+      <c r="C42">
+        <v>94.69</v>
       </c>
     </row>
     <row r="43" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A43" t="s">
-        <v>35</v>
+        <v>41</v>
       </c>
       <c r="B43">
-        <v>94.04</v>
+        <v>94.72</v>
       </c>
       <c r="C43">
-        <v>93.8</v>
+        <v>94.65</v>
       </c>
     </row>
     <row r="44" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A44" s="3" t="s">
-        <v>36</v>
-      </c>
-      <c r="B44">
-        <v>94.49</v>
-      </c>
-      <c r="C44">
-        <v>94.22</v>
+      <c r="A44" s="5" t="s">
+        <v>51</v>
       </c>
     </row>
     <row r="45" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A45" t="s">
-        <v>37</v>
+      <c r="A45" s="2" t="s">
+        <v>52</v>
       </c>
       <c r="B45">
-        <v>94.58</v>
+        <v>98.11</v>
       </c>
       <c r="C45">
-        <v>94.46</v>
+        <v>97</v>
       </c>
     </row>
     <row r="46" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A46" s="2" t="s">
-        <v>38</v>
+        <v>53</v>
       </c>
       <c r="B46">
-        <v>94.83</v>
+        <v>98.1</v>
       </c>
       <c r="C46">
-        <v>94.64</v>
+        <v>97.14</v>
       </c>
     </row>
     <row r="47" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A47" t="s">
-        <v>39</v>
+      <c r="A47" s="2" t="s">
+        <v>44</v>
       </c>
       <c r="B47">
-        <v>94.63</v>
+        <v>90.13</v>
       </c>
       <c r="C47">
-        <v>94.37</v>
+        <v>90.69</v>
       </c>
     </row>
     <row r="48" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A48" s="2" t="s">
-        <v>40</v>
+        <v>45</v>
       </c>
       <c r="B48">
-        <v>94.84</v>
+        <v>90.17</v>
       </c>
       <c r="C48">
-        <v>94.69</v>
-      </c>
-    </row>
-    <row r="50" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A50" t="s">
-        <v>41</v>
+        <v>90.83</v>
+      </c>
+    </row>
+    <row r="49" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A49" s="4" t="s">
+        <v>46</v>
+      </c>
+      <c r="B49">
+        <v>98.7</v>
+      </c>
+      <c r="C49">
+        <v>97.74</v>
+      </c>
+    </row>
+    <row r="50" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A50" s="4" t="s">
+        <v>48</v>
       </c>
       <c r="B50">
-        <v>94.72</v>
+        <v>98.72</v>
       </c>
       <c r="C50">
-        <v>94.65</v>
-      </c>
-    </row>
-    <row r="52" spans="1:3" x14ac:dyDescent="0.3">
+        <v>97.75</v>
+      </c>
+    </row>
+    <row r="51" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A51" s="2" t="s">
+        <v>50</v>
+      </c>
+      <c r="B51">
+        <v>98.73</v>
+      </c>
+      <c r="C51">
+        <v>97.38</v>
+      </c>
+    </row>
+    <row r="52" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A52" s="2" t="s">
-        <v>44</v>
+        <v>56</v>
       </c>
       <c r="B52">
-        <v>98.11</v>
+        <v>98.7</v>
       </c>
       <c r="C52">
-        <v>97</v>
-      </c>
-    </row>
-    <row r="53" spans="1:3" x14ac:dyDescent="0.3">
+        <v>97.78</v>
+      </c>
+    </row>
+    <row r="53" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A53" s="2" t="s">
-        <v>45</v>
+        <v>49</v>
       </c>
       <c r="B53">
-        <v>98.1</v>
+        <v>99.21</v>
       </c>
       <c r="C53">
-        <v>97.14</v>
-      </c>
-    </row>
-    <row r="55" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A55" s="2" t="s">
-        <v>46</v>
-      </c>
-      <c r="B55">
-        <v>90.13</v>
-      </c>
-      <c r="C55">
-        <v>90.69</v>
-      </c>
-    </row>
-    <row r="56" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A56" s="2" t="s">
-        <v>47</v>
-      </c>
-      <c r="B56">
-        <v>90.17</v>
-      </c>
-      <c r="C56">
-        <v>90.83</v>
+        <v>97.71</v>
+      </c>
+      <c r="D53" s="5" t="s">
+        <v>54</v>
+      </c>
+    </row>
+    <row r="54" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A54" s="2" t="s">
+        <v>55</v>
+      </c>
+      <c r="B54">
+        <v>98.7</v>
+      </c>
+      <c r="C54">
+        <v>97.82</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
PRACTICA 5: Cambios en los ficheros y memoria casi acabada
</commit_message>
<xml_diff>
--- a/practica5/resumen.xlsx
+++ b/practica5/resumen.xlsx
@@ -19,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="57" uniqueCount="57">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="59" uniqueCount="59">
   <si>
     <t>Modelo</t>
   </si>
@@ -190,6 +190,12 @@
   </si>
   <si>
     <t>Perceptron con 2 capas ocultas (100,100) 'relu,relu' y salida 'softmax' con batch = 16 dropout(0.2) y earlystop 3</t>
+  </si>
+  <si>
+    <t>Perceptron con capa oculta (500) 'relu' y salida 'softmax'</t>
+  </si>
+  <si>
+    <t>Perceptron con capa oculta (750) 'relu' y salida 'softmax'</t>
   </si>
 </sst>
 </file>
@@ -1014,15 +1020,15 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:D54"/>
+  <dimension ref="A1:D56"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A46" workbookViewId="0">
-      <selection activeCell="E58" sqref="E58"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="C15" sqref="C15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="99.88671875" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="48.44140625" customWidth="1"/>
     <col min="2" max="2" width="21.5546875" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="12.33203125" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="12.44140625" bestFit="1" customWidth="1"/>
@@ -1162,447 +1168,447 @@
     </row>
     <row r="13" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A13" t="s">
-        <v>11</v>
+        <v>57</v>
       </c>
       <c r="B13" s="1">
-        <v>92</v>
+        <v>93.86</v>
       </c>
       <c r="C13" s="1">
-        <v>92.04</v>
+        <v>93.87</v>
       </c>
     </row>
     <row r="14" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A14" t="s">
-        <v>12</v>
+        <v>58</v>
       </c>
       <c r="B14" s="1">
-        <v>92.15</v>
+        <v>94.12</v>
       </c>
       <c r="C14" s="1">
-        <v>92.12</v>
+        <v>94.13</v>
       </c>
     </row>
     <row r="15" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A15" t="s">
-        <v>13</v>
-      </c>
-      <c r="B15">
-        <v>92.31</v>
-      </c>
-      <c r="C15">
-        <v>92.46</v>
+        <v>11</v>
+      </c>
+      <c r="B15" s="1">
+        <v>92</v>
+      </c>
+      <c r="C15" s="1">
+        <v>92.04</v>
       </c>
     </row>
     <row r="16" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A16" t="s">
-        <v>14</v>
-      </c>
-      <c r="B16">
-        <v>92.44</v>
-      </c>
-      <c r="C16">
-        <v>92.64</v>
+        <v>12</v>
+      </c>
+      <c r="B16" s="1">
+        <v>92.15</v>
+      </c>
+      <c r="C16" s="1">
+        <v>92.12</v>
       </c>
     </row>
     <row r="17" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A17" t="s">
-        <v>15</v>
+        <v>13</v>
       </c>
       <c r="B17">
         <v>92.31</v>
       </c>
       <c r="C17">
-        <v>92.55</v>
+        <v>92.46</v>
       </c>
     </row>
     <row r="18" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A18" t="s">
-        <v>16</v>
+        <v>14</v>
       </c>
       <c r="B18">
-        <v>92.3</v>
+        <v>92.44</v>
       </c>
       <c r="C18">
-        <v>92.46</v>
+        <v>92.64</v>
       </c>
     </row>
     <row r="19" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A19" t="s">
-        <v>17</v>
+        <v>15</v>
       </c>
       <c r="B19">
-        <v>93.95</v>
+        <v>92.31</v>
       </c>
       <c r="C19">
-        <v>93.74</v>
+        <v>92.55</v>
       </c>
     </row>
     <row r="20" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A20" t="s">
-        <v>18</v>
+        <v>16</v>
       </c>
       <c r="B20">
-        <v>93.98</v>
+        <v>92.3</v>
       </c>
       <c r="C20">
-        <v>93.84</v>
+        <v>92.46</v>
       </c>
     </row>
     <row r="21" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A21" t="s">
-        <v>19</v>
+        <v>17</v>
       </c>
       <c r="B21">
-        <v>93.84</v>
+        <v>93.95</v>
       </c>
       <c r="C21">
-        <v>94.03</v>
+        <v>93.74</v>
       </c>
     </row>
     <row r="22" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A22" t="s">
-        <v>20</v>
+        <v>18</v>
       </c>
       <c r="B22">
-        <v>93.81</v>
+        <v>93.98</v>
       </c>
       <c r="C22">
-        <v>93.78</v>
+        <v>93.84</v>
       </c>
     </row>
     <row r="23" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A23" t="s">
-        <v>21</v>
+        <v>19</v>
       </c>
       <c r="B23">
-        <v>93.78</v>
+        <v>93.84</v>
       </c>
       <c r="C23">
-        <v>93.7</v>
+        <v>94.03</v>
       </c>
     </row>
     <row r="24" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A24" t="s">
-        <v>22</v>
+        <v>20</v>
       </c>
       <c r="B24">
-        <v>94.04</v>
+        <v>93.81</v>
       </c>
       <c r="C24">
-        <v>94.05</v>
+        <v>93.78</v>
       </c>
     </row>
     <row r="25" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A25" t="s">
-        <v>23</v>
+        <v>21</v>
       </c>
       <c r="B25">
-        <v>93.68</v>
+        <v>93.78</v>
       </c>
       <c r="C25">
-        <v>93.62</v>
+        <v>93.7</v>
       </c>
     </row>
     <row r="26" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A26" t="s">
-        <v>24</v>
+        <v>22</v>
       </c>
       <c r="B26">
-        <v>94.21</v>
+        <v>94.04</v>
       </c>
       <c r="C26">
-        <v>94.16</v>
+        <v>94.05</v>
       </c>
     </row>
     <row r="27" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A27" t="s">
-        <v>25</v>
+        <v>23</v>
       </c>
       <c r="B27">
-        <v>94.24</v>
+        <v>93.68</v>
       </c>
       <c r="C27">
-        <v>93.99</v>
+        <v>93.62</v>
       </c>
     </row>
     <row r="28" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A28" t="s">
-        <v>26</v>
+        <v>24</v>
       </c>
       <c r="B28">
-        <v>94.13</v>
+        <v>94.21</v>
       </c>
       <c r="C28">
-        <v>93.83</v>
+        <v>94.16</v>
       </c>
     </row>
     <row r="29" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A29" t="s">
-        <v>27</v>
+        <v>25</v>
       </c>
       <c r="B29">
-        <v>94.11</v>
+        <v>94.24</v>
       </c>
       <c r="C29">
-        <v>94.07</v>
+        <v>93.99</v>
       </c>
     </row>
     <row r="30" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A30" t="s">
-        <v>28</v>
+        <v>26</v>
       </c>
       <c r="B30">
-        <v>94.6</v>
+        <v>94.13</v>
       </c>
       <c r="C30">
-        <v>94.45</v>
+        <v>93.83</v>
       </c>
     </row>
     <row r="31" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A31" t="s">
-        <v>29</v>
+        <v>27</v>
       </c>
       <c r="B31">
-        <v>94.27</v>
+        <v>94.11</v>
       </c>
       <c r="C31">
-        <v>94.09</v>
+        <v>94.07</v>
       </c>
     </row>
     <row r="32" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A32" t="s">
-        <v>30</v>
+        <v>28</v>
       </c>
       <c r="B32">
-        <v>94.01</v>
+        <v>94.6</v>
       </c>
       <c r="C32">
-        <v>93.99</v>
+        <v>94.45</v>
       </c>
     </row>
     <row r="33" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A33" t="s">
-        <v>31</v>
+        <v>29</v>
       </c>
       <c r="B33">
-        <v>94.53</v>
+        <v>94.27</v>
       </c>
       <c r="C33">
-        <v>94.28</v>
+        <v>94.09</v>
       </c>
     </row>
     <row r="34" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A34" t="s">
-        <v>32</v>
+        <v>30</v>
       </c>
       <c r="B34">
-        <v>94.55</v>
+        <v>94.01</v>
       </c>
       <c r="C34">
-        <v>94.36</v>
+        <v>93.99</v>
       </c>
     </row>
     <row r="35" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A35" t="s">
-        <v>33</v>
+        <v>31</v>
       </c>
       <c r="B35">
-        <v>94.54</v>
+        <v>94.53</v>
       </c>
       <c r="C35">
-        <v>94.49</v>
+        <v>94.28</v>
       </c>
     </row>
     <row r="36" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A36" t="s">
-        <v>34</v>
+        <v>32</v>
       </c>
       <c r="B36">
         <v>94.55</v>
       </c>
       <c r="C36">
-        <v>94.44</v>
+        <v>94.36</v>
       </c>
     </row>
     <row r="37" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A37" t="s">
-        <v>35</v>
+        <v>33</v>
       </c>
       <c r="B37">
-        <v>94.04</v>
+        <v>94.54</v>
       </c>
       <c r="C37">
-        <v>93.8</v>
+        <v>94.49</v>
       </c>
     </row>
     <row r="38" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A38" s="2" t="s">
-        <v>36</v>
+      <c r="A38" t="s">
+        <v>34</v>
       </c>
       <c r="B38">
-        <v>94.49</v>
+        <v>94.55</v>
       </c>
       <c r="C38">
-        <v>94.22</v>
+        <v>94.44</v>
       </c>
     </row>
     <row r="39" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A39" t="s">
-        <v>37</v>
+        <v>35</v>
       </c>
       <c r="B39">
-        <v>94.58</v>
+        <v>94.04</v>
       </c>
       <c r="C39">
-        <v>94.46</v>
+        <v>93.8</v>
       </c>
     </row>
     <row r="40" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A40" s="4" t="s">
-        <v>38</v>
+      <c r="A40" s="2" t="s">
+        <v>36</v>
       </c>
       <c r="B40">
-        <v>94.83</v>
+        <v>94.49</v>
       </c>
       <c r="C40">
-        <v>94.64</v>
+        <v>94.22</v>
       </c>
     </row>
     <row r="41" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A41" t="s">
-        <v>39</v>
+        <v>37</v>
       </c>
       <c r="B41">
-        <v>94.63</v>
+        <v>94.58</v>
       </c>
       <c r="C41">
-        <v>94.37</v>
+        <v>94.46</v>
       </c>
     </row>
     <row r="42" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A42" s="4" t="s">
-        <v>40</v>
+        <v>38</v>
       </c>
       <c r="B42">
-        <v>94.84</v>
+        <v>94.83</v>
       </c>
       <c r="C42">
-        <v>94.69</v>
+        <v>94.64</v>
       </c>
     </row>
     <row r="43" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A43" t="s">
+        <v>39</v>
+      </c>
+      <c r="B43">
+        <v>94.63</v>
+      </c>
+      <c r="C43">
+        <v>94.37</v>
+      </c>
+    </row>
+    <row r="44" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A44" s="4" t="s">
+        <v>40</v>
+      </c>
+      <c r="B44">
+        <v>94.84</v>
+      </c>
+      <c r="C44">
+        <v>94.69</v>
+      </c>
+    </row>
+    <row r="45" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A45" t="s">
         <v>41</v>
       </c>
-      <c r="B43">
+      <c r="B45">
         <v>94.72</v>
       </c>
-      <c r="C43">
+      <c r="C45">
         <v>94.65</v>
       </c>
     </row>
-    <row r="44" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A44" s="5" t="s">
+    <row r="46" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A46" s="5" t="s">
         <v>51</v>
-      </c>
-    </row>
-    <row r="45" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A45" s="2" t="s">
-        <v>52</v>
-      </c>
-      <c r="B45">
-        <v>98.11</v>
-      </c>
-      <c r="C45">
-        <v>97</v>
-      </c>
-    </row>
-    <row r="46" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A46" s="2" t="s">
-        <v>53</v>
-      </c>
-      <c r="B46">
-        <v>98.1</v>
-      </c>
-      <c r="C46">
-        <v>97.14</v>
       </c>
     </row>
     <row r="47" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A47" s="2" t="s">
-        <v>44</v>
+        <v>52</v>
       </c>
       <c r="B47">
-        <v>90.13</v>
+        <v>98.11</v>
       </c>
       <c r="C47">
-        <v>90.69</v>
+        <v>97</v>
       </c>
     </row>
     <row r="48" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A48" s="2" t="s">
+        <v>53</v>
+      </c>
+      <c r="B48">
+        <v>98.1</v>
+      </c>
+      <c r="C48">
+        <v>97.14</v>
+      </c>
+    </row>
+    <row r="49" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A49" s="2" t="s">
+        <v>44</v>
+      </c>
+      <c r="B49">
+        <v>90.13</v>
+      </c>
+      <c r="C49">
+        <v>90.69</v>
+      </c>
+    </row>
+    <row r="50" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A50" s="2" t="s">
         <v>45</v>
       </c>
-      <c r="B48">
+      <c r="B50">
         <v>90.17</v>
       </c>
-      <c r="C48">
+      <c r="C50">
         <v>90.83</v>
       </c>
     </row>
-    <row r="49" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A49" s="4" t="s">
+    <row r="51" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A51" s="4" t="s">
         <v>46</v>
       </c>
-      <c r="B49">
+      <c r="B51">
         <v>98.7</v>
       </c>
-      <c r="C49">
+      <c r="C51">
         <v>97.74</v>
       </c>
     </row>
-    <row r="50" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A50" s="4" t="s">
+    <row r="52" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A52" s="4" t="s">
         <v>48</v>
       </c>
-      <c r="B50">
+      <c r="B52">
         <v>98.72</v>
       </c>
-      <c r="C50">
+      <c r="C52">
         <v>97.75</v>
-      </c>
-    </row>
-    <row r="51" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A51" s="2" t="s">
-        <v>50</v>
-      </c>
-      <c r="B51">
-        <v>98.73</v>
-      </c>
-      <c r="C51">
-        <v>97.38</v>
-      </c>
-    </row>
-    <row r="52" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A52" s="2" t="s">
-        <v>56</v>
-      </c>
-      <c r="B52">
-        <v>98.7</v>
-      </c>
-      <c r="C52">
-        <v>97.78</v>
       </c>
     </row>
     <row r="53" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A53" s="2" t="s">
-        <v>49</v>
+        <v>50</v>
       </c>
       <c r="B53">
-        <v>99.21</v>
+        <v>98.73</v>
       </c>
       <c r="C53">
-        <v>97.71</v>
+        <v>97.38</v>
       </c>
       <c r="D53" s="5" t="s">
         <v>54</v>
@@ -1610,12 +1616,34 @@
     </row>
     <row r="54" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A54" s="2" t="s">
-        <v>55</v>
+        <v>56</v>
       </c>
       <c r="B54">
         <v>98.7</v>
       </c>
       <c r="C54">
+        <v>97.78</v>
+      </c>
+    </row>
+    <row r="55" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A55" s="2" t="s">
+        <v>49</v>
+      </c>
+      <c r="B55">
+        <v>99.21</v>
+      </c>
+      <c r="C55">
+        <v>97.71</v>
+      </c>
+    </row>
+    <row r="56" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A56" s="2" t="s">
+        <v>55</v>
+      </c>
+      <c r="B56">
+        <v>98.7</v>
+      </c>
+      <c r="C56">
         <v>97.82</v>
       </c>
     </row>

</xml_diff>